<commit_message>
web 125 - final scores
</commit_message>
<xml_diff>
--- a/125/125.xlsx
+++ b/125/125.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MFT\004-scores\125\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alameheli\Desktop\scores\mft-scores\125\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061BE669-85D5-4272-B2DE-28FDA1BBB4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87DA318-AA54-49C4-B7CD-59741BFD823C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="web 125" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -579,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,15 +1541,15 @@
         <v>0</v>
       </c>
       <c r="D33" s="14">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E33" s="15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F33" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1593,15 +1595,15 @@
         <v>9</v>
       </c>
       <c r="D36" s="14">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="E36" s="15">
         <f>B36+C36+D36</f>
-        <v>47.137499999999996</v>
+        <v>102.13749999999999</v>
       </c>
       <c r="F36" s="16">
         <f>E36</f>
-        <v>47.137499999999996</v>
+        <v>102.13749999999999</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1616,15 +1618,15 @@
         <v>10</v>
       </c>
       <c r="D37" s="14">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E37" s="15">
         <f>B37+C37+D37</f>
-        <v>50.443750000000001</v>
+        <v>98.443749999999994</v>
       </c>
       <c r="F37" s="16">
         <f t="shared" ref="F37" si="2">E37</f>
-        <v>50.443750000000001</v>
+        <v>98.443749999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>